<commit_message>
vector norm for different models
перенес код(с расчетом нормы из мейна в отдельную функцию) для текущей задачи пока так сойдет, потом перепишу
</commit_message>
<xml_diff>
--- a/docs/misc/Results_of_testing_different_models.xlsx
+++ b/docs/misc/Results_of_testing_different_models.xlsx
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.073131322860718</v>
+        <v>3.307767391204834</v>
       </c>
     </row>
     <row r="3">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3.469616413116455</v>
+        <v>3.389590978622437</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5.170926570892334</v>
+        <v>5.408395290374756</v>
       </c>
     </row>
     <row r="5">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5.373730659484863</v>
+        <v>6.40941309928894</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.970797777175903</v>
+        <v>3.98141622543335</v>
       </c>
     </row>
     <row r="7">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4.083895683288574</v>
+        <v>4.376898050308228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>